<commit_message>
avances  14/04/2021  6.06  pm
</commit_message>
<xml_diff>
--- a/uploads/documentos/formato_filatelia.xlsx
+++ b/uploads/documentos/formato_filatelia.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>NUMERO</t>
   </si>
@@ -67,22 +67,13 @@
     <t>FOTO_VARIANTES_ERRORES</t>
   </si>
   <si>
-    <t>7de7a124-0d42-4199-bf86-773f7eabd52b</t>
-  </si>
-  <si>
-    <t>4e239eff-a193-4984-bf00-53793af67eff</t>
-  </si>
-  <si>
-    <t>e197ec02-a2ab-4741-8a38-025f0d55e7ae</t>
-  </si>
-  <si>
-    <t>70505115-a0b2-4f34-9b5f-fed1d124c42b</t>
-  </si>
-  <si>
-    <t>4ccf6e2e-9e0a-482b-9992-911facd312bf</t>
-  </si>
-  <si>
-    <t>fd61690a-54f2-48cb-916f-0a0f52422678</t>
+    <t>660a01bf-f5d1-4c64-a425-a565b0b58d0f</t>
+  </si>
+  <si>
+    <t>ecbffc84-d250-4920-a67c-458a116d3cf0</t>
+  </si>
+  <si>
+    <t>e6a69ea6-4172-437f-bb8e-9f0f91bf0e8f</t>
   </si>
 </sst>
 </file>
@@ -275,123 +266,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1333500" cy="1333500"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1333500" cy="1333500"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1333500" cy="1333500"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -717,7 +591,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -866,78 +740,6 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" ht="105" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-    </row>
-    <row r="6" ht="105" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-    </row>
-    <row r="7" ht="105" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>